<commit_message>
Update Smart Row Parent Partcode.xlsx
ok
</commit_message>
<xml_diff>
--- a/Smart Row Parent Partcode.xlsx
+++ b/Smart Row Parent Partcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vertivco-my.sharepoint.com/personal/sanket_bugade_vertivco_com/Documents/Documents/APP/my-streamlit-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{E78B3F63-4E7F-4CBF-8578-F9DEE28D0425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDC8EC27-1266-436F-B99D-53A2E1F5036C}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{E78B3F63-4E7F-4CBF-8578-F9DEE28D0425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C9398E6-0B59-41B2-809D-1382C5A4B2E0}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{9A64FB53-8709-49B2-BEC5-D0A2AC4A411D}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="238">
   <si>
     <t>Description</t>
   </si>
@@ -777,9 +777,6 @@
     <t>Subassembly, UPS O/P Distribution for SC1</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>LP</t>
   </si>
 </sst>
@@ -1000,16 +997,127 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="18">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1025,11 +1133,47 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1051,28 +1195,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1146,13 +1268,10 @@
       <sheetName val="VEPL_SMARTSOLUTION_DTP_INR"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0" refreshError="1">
         <row r="1">
           <cell r="C1" t="str">
             <v>Product Value</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v>Value</v>
           </cell>
         </row>
         <row r="2">
@@ -41929,14 +42048,18 @@
 </externalLink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3C7EDFF6-F4B1-46A1-AAAD-ACE3EF8BE9F3}" name="Table2" displayName="Table2" ref="A1:D57" totalsRowShown="0">
   <autoFilter ref="A1:D57" xr:uid="{3C7EDFF6-F4B1-46A1-AAAD-ACE3EF8BE9F3}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0201713B-365C-4E18-8B59-C82160436B08}" name="Item" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{0201713B-365C-4E18-8B59-C82160436B08}" name="Item" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{08C8D759-D663-4A0A-A4FE-296410B91C47}" name="Description"/>
     <tableColumn id="5" xr3:uid="{F7BC5DF1-245D-43E0-B9F8-29C3F764A98A}" name="Quantity"/>
-    <tableColumn id="8" xr3:uid="{28DE39ED-2F29-440C-953F-C1D0397D0FF7}" name="LP" dataDxfId="11">
+    <tableColumn id="8" xr3:uid="{28DE39ED-2F29-440C-953F-C1D0397D0FF7}" name="LP" dataDxfId="16">
       <calculatedColumnFormula array="1">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A2),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</calculatedColumnFormula>
     </tableColumn>
@@ -41946,13 +42069,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{904630A7-821A-466C-B09D-37A99E41F225}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{904630A7-821A-466C-B09D-37A99E41F225}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:D32" xr:uid="{904630A7-821A-466C-B09D-37A99E41F225}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4038F6B6-16E1-4211-9409-76961F84204D}" name="Item" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{E7AE195B-405C-4829-AFD2-4BFB04B154CE}" name="Description" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{C5D1E526-04E7-436C-AB26-908A94433498}" name="Quantity" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{1A55579C-A765-457B-BFB4-6EDF42CE7960}" name="LP" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{4038F6B6-16E1-4211-9409-76961F84204D}" name="Item" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E7AE195B-405C-4829-AFD2-4BFB04B154CE}" name="Description" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{C5D1E526-04E7-436C-AB26-908A94433498}" name="Quantity" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1A55579C-A765-457B-BFB4-6EDF42CE7960}" name="LP" dataDxfId="8">
       <calculatedColumnFormula array="1">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A2),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</calculatedColumnFormula>
     </tableColumn>
@@ -41962,16 +42085,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{37E12B78-64AE-47CC-B5F7-6E1EAE944EAE}" name="Table3" displayName="Table3" ref="A1:E84" totalsRowShown="0">
-  <autoFilter ref="A1:E84" xr:uid="{37E12B78-64AE-47CC-B5F7-6E1EAE944EAE}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{81DDDFA8-5FA1-4775-959B-874DA3901688}" name="Item" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{172E9D6C-E1E8-4513-8672-E3AF6DE2CC8A}" name="Description" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{E7317290-3C07-49D3-ABAC-C9434807AAAC}" name="Quantity"/>
-    <tableColumn id="6" xr3:uid="{D3AB9579-4424-40E5-BB9F-389A488836AA}" name="Column1" dataDxfId="5">
-      <calculatedColumnFormula>_xlfn.XLOOKUP(A2, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{6AF05084-ECFE-4A9A-A5DD-49C06A4BD591}" name="LP">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{37E12B78-64AE-47CC-B5F7-6E1EAE944EAE}" name="Table3" displayName="Table3" ref="A1:D84" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:D84" xr:uid="{37E12B78-64AE-47CC-B5F7-6E1EAE944EAE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{81DDDFA8-5FA1-4775-959B-874DA3901688}" name="Item" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{172E9D6C-E1E8-4513-8672-E3AF6DE2CC8A}" name="Description" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E7317290-3C07-49D3-ABAC-C9434807AAAC}" name="Quantity" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{6AF05084-ECFE-4A9A-A5DD-49C06A4BD591}" name="LP" dataDxfId="1">
       <calculatedColumnFormula array="1">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A2),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</calculatedColumnFormula>
     </tableColumn>
@@ -42821,7 +42941,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42842,7 +42962,7 @@
         <v>130</v>
       </c>
       <c r="D1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -43749,7 +43869,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43771,7 +43891,7 @@
         <v>130</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -44275,10 +44395,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC62E752-F41D-43AD-801E-2D8B3E88FABD}">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I87" sqref="I87"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44286,1675 +44406,1339 @@
     <col min="1" max="1" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="113.6640625" style="22" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="0.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="E1" t="s">
-        <v>238</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
         <v>850000100000</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="9">
         <v>2</v>
       </c>
-      <c r="D2" s="13">
-        <f>_xlfn.XLOOKUP(A2, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>529947.51139999996</v>
-      </c>
-      <c r="E2" cm="1">
-        <f t="array" ref="E2">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A2),
+      <c r="D2" s="11" cm="1">
+        <f t="array" ref="D2">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A2),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>583783.10710000002</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>325721000000</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
         <v>1</v>
       </c>
-      <c r="D3">
-        <f>_xlfn.XLOOKUP(A3, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>186147.2445</v>
-      </c>
-      <c r="E3" cm="1">
-        <f t="array" ref="E3">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A3),
+      <c r="D3" s="11" cm="1">
+        <f t="array" ref="D3">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A3),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>204053</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
         <v>325720000000</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="9">
         <v>1</v>
       </c>
-      <c r="D4">
-        <f>_xlfn.XLOOKUP(A4, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>110346.6</v>
-      </c>
-      <c r="E4" cm="1">
-        <f t="array" ref="E4">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A4),
+      <c r="D4" s="11" cm="1">
+        <f t="array" ref="D4">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A4),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>75131.8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>325721000001</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>1</v>
       </c>
-      <c r="D5">
-        <f>_xlfn.XLOOKUP(A5, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>112646.8636</v>
-      </c>
-      <c r="E5" cm="1">
-        <f t="array" ref="E5">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A5),
+      <c r="D5" s="11" cm="1">
+        <f t="array" ref="D5">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A5),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>140833</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
         <v>325703000017</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6">
-        <f>_xlfn.XLOOKUP(A6, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>261912</v>
-      </c>
-      <c r="E6" cm="1">
-        <f t="array" ref="E6">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A6),
+      <c r="D6" s="11" cm="1">
+        <f t="array" ref="D6">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A6),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>386203</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
         <v>325723000000</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7">
-        <f>_xlfn.XLOOKUP(A7, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>6379.8</v>
-      </c>
-      <c r="E7" cm="1">
-        <f t="array" ref="E7">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A7),
+      <c r="D7" s="11" cm="1">
+        <f t="array" ref="D7">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A7),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>6683.6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
         <v>681000071600</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="9">
         <v>4</v>
       </c>
-      <c r="D8">
-        <f>_xlfn.XLOOKUP(A8, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>34540</v>
-      </c>
-      <c r="E8" cm="1">
-        <f t="array" ref="E8">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A8),
+      <c r="D8" s="11" cm="1">
+        <f t="array" ref="D8">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A8),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>34540</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>325722000000</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <f>_xlfn.XLOOKUP(A9, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>405986.7</v>
-      </c>
-      <c r="E9" cm="1">
-        <f t="array" ref="E9">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A9),
+      <c r="D9" s="11" cm="1">
+        <f t="array" ref="D9">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A9),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>233919.4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
         <v>325722000001</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="9">
         <v>1</v>
       </c>
-      <c r="D10">
-        <f>_xlfn.XLOOKUP(A10, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>309586.13699999999</v>
-      </c>
-      <c r="E10" cm="1">
-        <f t="array" ref="E10">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A10),
+      <c r="D10" s="11" cm="1">
+        <f t="array" ref="D10">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A10),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>334400</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>325707000003</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11">
-        <f>_xlfn.XLOOKUP(A11, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>114961</v>
-      </c>
-      <c r="E11" cm="1">
-        <f t="array" ref="E11">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A11),
+      <c r="D11" s="11" cm="1">
+        <f t="array" ref="D11">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A11),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>114961</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <v>325707000005</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12">
-        <f>_xlfn.XLOOKUP(A12, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>122061.34600000001</v>
-      </c>
-      <c r="E12" cm="1">
-        <f t="array" ref="E12">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A12),
+      <c r="D12" s="11" cm="1">
+        <f t="array" ref="D12">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A12),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>122061.34600000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
         <v>125004000018</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="9">
         <v>4</v>
       </c>
-      <c r="D13">
-        <f>_xlfn.XLOOKUP(A13, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>2625</v>
-      </c>
-      <c r="E13" cm="1">
-        <f t="array" ref="E13">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A13),
+      <c r="D13" s="11" cm="1">
+        <f t="array" ref="D13">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A13),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>5253.6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
         <v>125004000037</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="9">
         <v>4</v>
       </c>
-      <c r="D14">
-        <f>_xlfn.XLOOKUP(A14, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>3969</v>
-      </c>
-      <c r="E14" cm="1">
-        <f t="array" ref="E14">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A14),
+      <c r="D14" s="11" cm="1">
+        <f t="array" ref="D14">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A14),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>6279</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
         <v>125300000126</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="9">
         <v>4</v>
       </c>
-      <c r="D15">
-        <f>_xlfn.XLOOKUP(A15, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>29820</v>
-      </c>
-      <c r="E15" cm="1">
-        <f t="array" ref="E15">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A15),
+      <c r="D15" s="11" cm="1">
+        <f t="array" ref="D15">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A15),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>64767</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
         <v>492100639040</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16">
-        <f>_xlfn.XLOOKUP(A16, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>35236.844989999998</v>
-      </c>
-      <c r="E16" cm="1">
-        <f t="array" ref="E16">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A16),
+      <c r="D16" s="11" cm="1">
+        <f t="array" ref="D16">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A16),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>42702</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
         <v>325705000033</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="9">
         <v>3</v>
       </c>
-      <c r="D17">
-        <f>_xlfn.XLOOKUP(A17, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>9500.2161950000009</v>
-      </c>
-      <c r="E17" cm="1">
-        <f t="array" ref="E17">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A17),
+      <c r="D17" s="11" cm="1">
+        <f t="array" ref="D17">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A17),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>13050</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
         <v>325715000000</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="9">
         <v>1</v>
       </c>
-      <c r="D18">
-        <f>_xlfn.XLOOKUP(A18, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>11220</v>
-      </c>
-      <c r="E18" cm="1">
-        <f t="array" ref="E18">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A18),
+      <c r="D18" s="11" cm="1">
+        <f t="array" ref="D18">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A18),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>11220</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
         <v>325715000001</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="9">
         <v>1</v>
       </c>
-      <c r="D19">
-        <f>_xlfn.XLOOKUP(A19, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>31640.400000000001</v>
-      </c>
-      <c r="E19" cm="1">
-        <f t="array" ref="E19">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A19),
+      <c r="D19" s="11" cm="1">
+        <f t="array" ref="D19">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A19),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>31640.400000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="8">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
         <v>325715000002</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="9">
         <v>1</v>
       </c>
-      <c r="D20">
-        <f>_xlfn.XLOOKUP(A20, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>37620</v>
-      </c>
-      <c r="E20" cm="1">
-        <f t="array" ref="E20">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A20),
+      <c r="D20" s="11" cm="1">
+        <f t="array" ref="D20">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A20),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>37620</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
         <v>325715000003</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="9">
         <v>1</v>
       </c>
-      <c r="D21">
-        <f>_xlfn.XLOOKUP(A21, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>103788.39780000001</v>
-      </c>
-      <c r="E21" cm="1">
-        <f t="array" ref="E21">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A21),
+      <c r="D21" s="11" cm="1">
+        <f t="array" ref="D21">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A21),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>97608</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="8">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
         <v>170893010359</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="9">
         <v>1</v>
       </c>
-      <c r="D22">
-        <f>_xlfn.XLOOKUP(A22, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>168</v>
-      </c>
-      <c r="E22" cm="1">
-        <f t="array" ref="E22">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A22),
+      <c r="D22" s="11" cm="1">
+        <f t="array" ref="D22">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A22),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="8">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
         <v>340101070019</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="9">
         <v>1</v>
       </c>
-      <c r="D23">
-        <f>_xlfn.XLOOKUP(A23, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>1930.180521</v>
-      </c>
-      <c r="E23" cm="1">
-        <f t="array" ref="E23">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A23),
+      <c r="D23" s="11" cm="1">
+        <f t="array" ref="D23">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A23),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>2562</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="8">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
         <v>325705000104</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="9">
         <v>1</v>
       </c>
-      <c r="D24" t="str">
-        <f>_xlfn.XLOOKUP(A24, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>Not Found</v>
-      </c>
-      <c r="E24">
+      <c r="D24" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="8">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
         <v>325705000003</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="9">
         <v>1</v>
       </c>
-      <c r="D25">
-        <f>_xlfn.XLOOKUP(A25, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>557840.80000000005</v>
-      </c>
-      <c r="E25" cm="1">
-        <f t="array" ref="E25">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A25),
+      <c r="D25" s="11" cm="1">
+        <f t="array" ref="D25">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A25),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>557840.80000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="8">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
         <v>325724210202</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="9">
         <v>1</v>
       </c>
-      <c r="D26">
-        <f>_xlfn.XLOOKUP(A26, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>1823978.1</v>
-      </c>
-      <c r="E26" cm="1">
-        <f t="array" ref="E26">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A26),
+      <c r="D26" s="11" cm="1">
+        <f t="array" ref="D26">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A26),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>1804486.33</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="8">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
         <v>325703000021</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="9">
         <v>1</v>
       </c>
-      <c r="D27">
-        <f>_xlfn.XLOOKUP(A27, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>120970.5</v>
-      </c>
-      <c r="E27" cm="1">
-        <f t="array" ref="E27">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A27),
+      <c r="D27" s="11" cm="1">
+        <f t="array" ref="D27">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A27),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>164078</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="8">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
         <v>325722000015</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="9">
         <v>1</v>
       </c>
-      <c r="D28">
-        <f>_xlfn.XLOOKUP(A28, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>128249</v>
-      </c>
-      <c r="E28" cm="1">
-        <f t="array" ref="E28">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A28),
+      <c r="D28" s="11" cm="1">
+        <f t="array" ref="D28">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A28),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>128249</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="9">
         <v>1</v>
       </c>
-      <c r="D29" t="str">
-        <f>_xlfn.XLOOKUP(A29, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>Not Found</v>
-      </c>
-      <c r="E29">
+      <c r="D29" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="8">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
         <v>325705000118</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="9">
         <v>1</v>
       </c>
-      <c r="D30">
-        <f>_xlfn.XLOOKUP(A30, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>526801</v>
-      </c>
-      <c r="E30" cm="1">
-        <f t="array" ref="E30">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A30),
+      <c r="D30" s="11" cm="1">
+        <f t="array" ref="D30">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A30),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>646775</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="8">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="10">
         <v>325701000013</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="9">
         <v>1</v>
       </c>
-      <c r="D31">
-        <f>_xlfn.XLOOKUP(A31, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>84603.199999999997</v>
-      </c>
-      <c r="E31" cm="1">
-        <f t="array" ref="E31">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A31),
+      <c r="D31" s="11" cm="1">
+        <f t="array" ref="D31">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A31),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>84603.199999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="8">
+    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="10">
         <v>325720000001</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="9">
         <v>1</v>
       </c>
-      <c r="D32">
-        <f>_xlfn.XLOOKUP(A32, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>161020.20000000001</v>
-      </c>
-      <c r="E32" cm="1">
-        <f t="array" ref="E32">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A32),
+      <c r="D32" s="11" cm="1">
+        <f t="array" ref="D32">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A32),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>161020.20000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="8">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="10">
         <v>325705000165</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="9">
         <v>1</v>
       </c>
-      <c r="D33">
-        <f>_xlfn.XLOOKUP(A33, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>726801</v>
-      </c>
-      <c r="E33" cm="1">
-        <f t="array" ref="E33">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A33),
+      <c r="D33" s="11" cm="1">
+        <f t="array" ref="D33">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A33),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>753887.5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="8">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="10">
         <v>325705000073</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="9">
         <v>1</v>
       </c>
-      <c r="D34">
-        <f>_xlfn.XLOOKUP(A34, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>103510</v>
-      </c>
-      <c r="E34" cm="1">
-        <f t="array" ref="E34">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A34),
+      <c r="D34" s="11" cm="1">
+        <f t="array" ref="D34">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A34),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>103510</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="8">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="10">
         <v>325720000068</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="9">
         <v>1</v>
       </c>
-      <c r="D35">
-        <f>_xlfn.XLOOKUP(A35, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>103599.8</v>
-      </c>
-      <c r="E35" cm="1">
-        <f t="array" ref="E35">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A35),
+      <c r="D35" s="11" cm="1">
+        <f t="array" ref="D35">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A35),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>103599.8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="8">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="10">
         <v>850000100004</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="9">
         <v>1</v>
       </c>
-      <c r="D36">
-        <f>_xlfn.XLOOKUP(A36, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>552000</v>
-      </c>
-      <c r="E36" cm="1">
-        <f t="array" ref="E36">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A36),
+      <c r="D36" s="11" cm="1">
+        <f t="array" ref="D36">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A36),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>1079603</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="8">
+    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="10">
         <v>325707000087</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="9">
         <v>1</v>
       </c>
-      <c r="D37">
-        <f>_xlfn.XLOOKUP(A37, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>136228</v>
-      </c>
-      <c r="E37" cm="1">
-        <f t="array" ref="E37">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A37),
+      <c r="D37" s="11" cm="1">
+        <f t="array" ref="D37">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A37),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>136228</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="8">
+    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="10">
         <v>325707000088</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="9">
         <v>1</v>
       </c>
-      <c r="D38">
-        <f>_xlfn.XLOOKUP(A38, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>99827</v>
-      </c>
-      <c r="E38" cm="1">
-        <f t="array" ref="E38">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A38),
+      <c r="D38" s="11" cm="1">
+        <f t="array" ref="D38">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A38),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>99827</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="8">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="10">
         <v>325712000027</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="9">
         <v>1</v>
       </c>
-      <c r="D39">
-        <f>_xlfn.XLOOKUP(A39, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>77994</v>
-      </c>
-      <c r="E39" cm="1">
-        <f t="array" ref="E39">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A39),
+      <c r="D39" s="11" cm="1">
+        <f t="array" ref="D39">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A39),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>77994</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="8">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="10">
         <v>325707000017</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="9">
         <v>1</v>
       </c>
-      <c r="D40">
-        <f>_xlfn.XLOOKUP(A40, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>10865.8</v>
-      </c>
-      <c r="E40" cm="1">
-        <f t="array" ref="E40">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A40),
+      <c r="D40" s="11" cm="1">
+        <f t="array" ref="D40">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A40),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>10865.8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="8">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="10">
         <v>325712000008</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="9">
         <v>1</v>
       </c>
-      <c r="D41">
-        <f>_xlfn.XLOOKUP(A41, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>7418.4</v>
-      </c>
-      <c r="E41" cm="1">
-        <f t="array" ref="E41">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A41),
+      <c r="D41" s="11" cm="1">
+        <f t="array" ref="D41">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A41),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>7418.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="8">
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="10">
         <v>325707000085</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="9">
         <v>1</v>
       </c>
-      <c r="D42">
-        <f>_xlfn.XLOOKUP(A42, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>135317</v>
-      </c>
-      <c r="E42" cm="1">
-        <f t="array" ref="E42">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A42),
+      <c r="D42" s="11" cm="1">
+        <f t="array" ref="D42">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A42),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>135317</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="8">
+    <row r="43" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="10">
         <v>325707000086</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="9">
         <v>1</v>
       </c>
-      <c r="D43">
-        <f>_xlfn.XLOOKUP(A43, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>156941</v>
-      </c>
-      <c r="E43" cm="1">
-        <f t="array" ref="E43">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A43),
+      <c r="D43" s="11" cm="1">
+        <f t="array" ref="D43">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A43),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>156941</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="8">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="10">
         <v>325707000018</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="9">
         <v>1</v>
       </c>
-      <c r="D44">
-        <f>_xlfn.XLOOKUP(A44, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>10692</v>
-      </c>
-      <c r="E44" cm="1">
-        <f t="array" ref="E44">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A44),
+      <c r="D44" s="11" cm="1">
+        <f t="array" ref="D44">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A44),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>10692</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="8">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="10">
         <v>325706000076</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="9">
         <v>1</v>
       </c>
-      <c r="D45">
-        <f>_xlfn.XLOOKUP(A45, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>11000</v>
-      </c>
-      <c r="E45" cm="1">
-        <f t="array" ref="E45">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A45),
+      <c r="D45" s="11" cm="1">
+        <f t="array" ref="D45">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A45),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>11000</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="8">
+    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="10">
         <v>325702000043</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="9">
         <v>1</v>
       </c>
-      <c r="D46">
-        <f>_xlfn.XLOOKUP(A46, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>4070</v>
-      </c>
-      <c r="E46" cm="1">
-        <f t="array" ref="E46">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A46),
+      <c r="D46" s="11" cm="1">
+        <f t="array" ref="D46">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A46),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>6141</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="8">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="10">
         <v>325715000033</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="9">
         <v>1</v>
       </c>
-      <c r="D47">
-        <f>_xlfn.XLOOKUP(A47, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>55755</v>
-      </c>
-      <c r="E47" cm="1">
-        <f t="array" ref="E47">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A47),
+      <c r="D47" s="11" cm="1">
+        <f t="array" ref="D47">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A47),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>78057</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="8">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="10">
         <v>200411300049</v>
       </c>
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="9">
         <v>1</v>
       </c>
-      <c r="D48">
-        <f>_xlfn.XLOOKUP(A48, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>14300</v>
-      </c>
-      <c r="E48" cm="1">
-        <f t="array" ref="E48">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A48),
+      <c r="D48" s="11" cm="1">
+        <f t="array" ref="D48">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A48),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>14300</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="8">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="10">
         <v>200402043000</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="9">
         <v>1</v>
       </c>
-      <c r="D49">
-        <f>_xlfn.XLOOKUP(A49, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>23876.82</v>
-      </c>
-      <c r="E49" cm="1">
-        <f t="array" ref="E49">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A49),
+      <c r="D49" s="11" cm="1">
+        <f t="array" ref="D49">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A49),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>23876.82</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="8">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="10">
         <v>325706000049</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="9">
         <v>1</v>
       </c>
-      <c r="D50">
-        <f>_xlfn.XLOOKUP(A50, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>15063.4</v>
-      </c>
-      <c r="E50" cm="1">
-        <f t="array" ref="E50">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A50),
+      <c r="D50" s="11" cm="1">
+        <f t="array" ref="D50">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A50),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>23622</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="8">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="10">
         <v>121663000047</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="9">
         <v>1</v>
       </c>
-      <c r="D51">
-        <f>_xlfn.XLOOKUP(A51, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>23315.599999999999</v>
-      </c>
-      <c r="E51" cm="1">
-        <f t="array" ref="E51">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A51),
+      <c r="D51" s="11" cm="1">
+        <f t="array" ref="D51">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A51),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>23315.599999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="8">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="10">
         <v>122310000075</v>
       </c>
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="9">
         <v>1</v>
       </c>
-      <c r="D52">
-        <f>_xlfn.XLOOKUP(A52, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>19399.599999999999</v>
-      </c>
-      <c r="E52" cm="1">
-        <f t="array" ref="E52">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A52),
+      <c r="D52" s="11" cm="1">
+        <f t="array" ref="D52">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A52),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>19399.599999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="8">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="10">
         <v>122310000571</v>
       </c>
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="9">
         <v>1</v>
       </c>
-      <c r="D53">
-        <f>_xlfn.XLOOKUP(A53, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>70</v>
-      </c>
-      <c r="E53" cm="1">
-        <f t="array" ref="E53">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A53),
+      <c r="D53" s="11" cm="1">
+        <f t="array" ref="D53">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A53),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="8">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="10">
         <v>170880002708</v>
       </c>
-      <c r="B54" s="22" t="s">
+      <c r="B54" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="9">
         <v>1</v>
       </c>
-      <c r="D54" t="str">
-        <f>_xlfn.XLOOKUP(A54, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>Not Found</v>
-      </c>
-      <c r="E54">
+      <c r="D54" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="8">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="10">
         <v>122120000049</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="9">
         <v>1</v>
       </c>
-      <c r="D55">
-        <f>_xlfn.XLOOKUP(A55, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>19</v>
-      </c>
-      <c r="E55" cm="1">
-        <f t="array" ref="E55">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A55),
+      <c r="D55" s="11" cm="1">
+        <f t="array" ref="D55">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A55),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="8">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="10">
         <v>274041010001</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="9">
         <v>2</v>
       </c>
-      <c r="D56">
-        <f>_xlfn.XLOOKUP(A56, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>786</v>
-      </c>
-      <c r="E56" cm="1">
-        <f t="array" ref="E56">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A56),
+      <c r="D56" s="11" cm="1">
+        <f t="array" ref="D56">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A56),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>786</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="8">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="10">
         <v>325723000004</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="9">
         <v>1</v>
       </c>
-      <c r="D57">
-        <f>_xlfn.XLOOKUP(A57, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>5861.1</v>
-      </c>
-      <c r="E57" cm="1">
-        <f t="array" ref="E57">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A57),
+      <c r="D57" s="11" cm="1">
+        <f t="array" ref="D57">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A57),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>18285</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="8">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="10">
         <v>354200030701</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="9">
         <v>1</v>
       </c>
-      <c r="D58">
-        <f>_xlfn.XLOOKUP(A58, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>169127.2</v>
-      </c>
-      <c r="E58" cm="1">
-        <f t="array" ref="E58">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A58),
+      <c r="D58" s="11" cm="1">
+        <f t="array" ref="D58">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A58),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>178251</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="8">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="10">
         <v>775110504801</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="9">
         <v>1</v>
       </c>
-      <c r="D59">
-        <f>_xlfn.XLOOKUP(A59, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>32370.799999999999</v>
-      </c>
-      <c r="E59" cm="1">
-        <f t="array" ref="E59">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A59),
+      <c r="D59" s="11" cm="1">
+        <f t="array" ref="D59">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A59),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>32370.799999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="8">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="10">
         <v>124301500000</v>
       </c>
-      <c r="B60" s="22" t="s">
+      <c r="B60" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="9">
         <v>1</v>
       </c>
-      <c r="D60">
-        <f>_xlfn.XLOOKUP(A60, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>67456.399999999994</v>
-      </c>
-      <c r="E60" cm="1">
-        <f t="array" ref="E60">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A60),
+      <c r="D60" s="11" cm="1">
+        <f t="array" ref="D60">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A60),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>67456.399999999994</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="8">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="10">
         <v>400500500068</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="9">
         <v>1</v>
       </c>
-      <c r="D61">
-        <f>_xlfn.XLOOKUP(A61, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>8855.0159729999996</v>
-      </c>
-      <c r="E61" cm="1">
-        <f t="array" ref="E61">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A61),
+      <c r="D61" s="11" cm="1">
+        <f t="array" ref="D61">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A61),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>16000</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="8">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="10">
         <v>42201001190</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="9">
         <v>1</v>
       </c>
-      <c r="D62">
-        <f>_xlfn.XLOOKUP(A62, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>124.090538</v>
-      </c>
-      <c r="E62" cm="1">
-        <f t="array" ref="E62">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A62),
+      <c r="D62" s="11" cm="1">
+        <f t="array" ref="D62">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A62),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>124.090538</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="8">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="10">
         <v>504215079000</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="9">
         <v>1</v>
       </c>
-      <c r="D63">
-        <f>_xlfn.XLOOKUP(A63, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>340397.2</v>
-      </c>
-      <c r="E63" cm="1">
-        <f t="array" ref="E63">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A63),
+      <c r="D63" s="11" cm="1">
+        <f t="array" ref="D63">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A63),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>936150</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="8">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="10">
         <v>34000420342</v>
       </c>
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="9">
         <v>1</v>
       </c>
-      <c r="D64">
-        <f>_xlfn.XLOOKUP(A64, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>11000</v>
-      </c>
-      <c r="E64" cm="1">
-        <f t="array" ref="E64">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A64),
+      <c r="D64" s="11" cm="1">
+        <f t="array" ref="D64">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A64),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>11000</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="8">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="10">
         <v>32404002010</v>
       </c>
-      <c r="B65" s="22" t="s">
+      <c r="B65" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="9">
         <v>1</v>
       </c>
-      <c r="D65">
-        <f>_xlfn.XLOOKUP(A65, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>14760</v>
-      </c>
-      <c r="E65" cm="1">
-        <f t="array" ref="E65">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A65),
+      <c r="D65" s="11" cm="1">
+        <f t="array" ref="D65">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A65),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>14760</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="8">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="10">
         <v>271921004221</v>
       </c>
-      <c r="B66" s="22" t="s">
+      <c r="B66" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="9">
         <v>1</v>
       </c>
-      <c r="D66">
-        <f>_xlfn.XLOOKUP(A66, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>2600</v>
-      </c>
-      <c r="E66" cm="1">
-        <f t="array" ref="E66">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A66),
+      <c r="D66" s="11" cm="1">
+        <f t="array" ref="D66">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A66),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>2600</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="8">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="10">
         <v>124300630001</v>
       </c>
-      <c r="B67" s="22" t="s">
+      <c r="B67" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="9">
         <v>1</v>
       </c>
-      <c r="D67">
-        <f>_xlfn.XLOOKUP(A67, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>6500</v>
-      </c>
-      <c r="E67" cm="1">
-        <f t="array" ref="E67">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A67),
+      <c r="D67" s="11" cm="1">
+        <f t="array" ref="D67">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A67),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>6500</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="8">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="10">
         <v>84607000001</v>
       </c>
-      <c r="B68" s="22" t="s">
+      <c r="B68" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="9">
         <v>1</v>
       </c>
-      <c r="D68">
-        <f>_xlfn.XLOOKUP(A68, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>85.8</v>
-      </c>
-      <c r="E68" cm="1">
-        <f t="array" ref="E68">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A68),
+      <c r="D68" s="11" cm="1">
+        <f t="array" ref="D68">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A68),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>94.08</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="8">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="10">
         <v>42200601190</v>
       </c>
-      <c r="B69" s="22" t="s">
+      <c r="B69" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="9">
         <v>1</v>
       </c>
-      <c r="D69">
-        <f>_xlfn.XLOOKUP(A69, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>80.096103999999997</v>
-      </c>
-      <c r="E69" cm="1">
-        <f t="array" ref="E69">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A69),
+      <c r="D69" s="11" cm="1">
+        <f t="array" ref="D69">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A69),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="8">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="10">
         <v>325701000065</v>
       </c>
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="9">
         <v>1</v>
       </c>
-      <c r="D70">
-        <f>_xlfn.XLOOKUP(A70, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>263235</v>
-      </c>
-      <c r="E70" cm="1">
-        <f t="array" ref="E70">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A70),
+      <c r="D70" s="11" cm="1">
+        <f t="array" ref="D70">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A70),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>408500</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="8">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="10">
         <v>325703000022</v>
       </c>
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="9">
         <v>1</v>
       </c>
-      <c r="D71">
-        <f>_xlfn.XLOOKUP(A71, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>138392.1</v>
-      </c>
-      <c r="E71" cm="1">
-        <f t="array" ref="E71">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A71),
+      <c r="D71" s="11" cm="1">
+        <f t="array" ref="D71">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A71),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>192678</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="8">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="10">
         <v>271921004218</v>
       </c>
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="9">
         <v>1</v>
       </c>
-      <c r="D72">
-        <f>_xlfn.XLOOKUP(A72, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>2600</v>
-      </c>
-      <c r="E72" cm="1">
-        <f t="array" ref="E72">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A72),
+      <c r="D72" s="11" cm="1">
+        <f t="array" ref="D72">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A72),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>2600</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="8">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="10">
         <v>280300633200</v>
       </c>
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="9">
         <v>1</v>
       </c>
-      <c r="D73">
-        <f>_xlfn.XLOOKUP(A73, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>1304.5999999999999</v>
-      </c>
-      <c r="E73" cm="1">
-        <f t="array" ref="E73">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A73),
+      <c r="D73" s="11" cm="1">
+        <f t="array" ref="D73">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A73),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>2531</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="8">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="10">
         <v>325703000029</v>
       </c>
-      <c r="B74" s="22" t="s">
+      <c r="B74" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="9">
         <v>1</v>
       </c>
-      <c r="D74">
-        <f>_xlfn.XLOOKUP(A74, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>158475</v>
-      </c>
-      <c r="E74" cm="1">
-        <f t="array" ref="E74">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A74),
+      <c r="D74" s="11" cm="1">
+        <f t="array" ref="D74">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A74),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>158475</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="8">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="10">
         <v>325703000035</v>
       </c>
-      <c r="B75" s="22" t="s">
+      <c r="B75" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="9">
         <v>1</v>
       </c>
-      <c r="D75">
-        <f>_xlfn.XLOOKUP(A75, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>307150</v>
-      </c>
-      <c r="E75" cm="1">
-        <f t="array" ref="E75">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A75),
+      <c r="D75" s="11" cm="1">
+        <f t="array" ref="D75">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A75),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>307150</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="8">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="10">
         <v>402001000938</v>
       </c>
-      <c r="B76" s="22" t="s">
+      <c r="B76" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="9">
         <v>1</v>
       </c>
-      <c r="D76">
-        <f>_xlfn.XLOOKUP(A76, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>48523</v>
-      </c>
-      <c r="E76" cm="1">
-        <f t="array" ref="E76">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A76),
+      <c r="D76" s="11" cm="1">
+        <f t="array" ref="D76">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A76),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>48523</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="8">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="10">
         <v>34000420321</v>
       </c>
-      <c r="B77" s="22" t="s">
+      <c r="B77" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="9">
         <v>1</v>
       </c>
-      <c r="D77">
-        <f>_xlfn.XLOOKUP(A77, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>6956.4</v>
-      </c>
-      <c r="E77" cm="1">
-        <f t="array" ref="E77">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A77),
+      <c r="D77" s="11" cm="1">
+        <f t="array" ref="D77">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A77),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>10062</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="8">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="10">
         <v>325723000002</v>
       </c>
-      <c r="B78" s="22" t="s">
+      <c r="B78" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="9">
         <v>1</v>
       </c>
-      <c r="D78">
-        <f>_xlfn.XLOOKUP(A78, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>5317.2</v>
-      </c>
-      <c r="E78" cm="1">
-        <f t="array" ref="E78">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A78),
+      <c r="D78" s="11" cm="1">
+        <f t="array" ref="D78">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A78),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>5570.4</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="8">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="10">
         <v>325721000028</v>
       </c>
-      <c r="B79" s="22" t="s">
+      <c r="B79" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="9">
         <v>1</v>
       </c>
-      <c r="D79">
-        <f>_xlfn.XLOOKUP(A79, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>30389</v>
-      </c>
-      <c r="E79" cm="1">
-        <f t="array" ref="E79">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A79),
+      <c r="D79" s="11" cm="1">
+        <f t="array" ref="D79">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A79),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>30389</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="8">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="10">
         <v>34000260335</v>
       </c>
-      <c r="B80" s="22" t="s">
+      <c r="B80" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="9">
         <v>1</v>
       </c>
-      <c r="D80">
-        <f>_xlfn.XLOOKUP(A80, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>6600</v>
-      </c>
-      <c r="E80" cm="1">
-        <f t="array" ref="E80">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A80),
+      <c r="D80" s="11" cm="1">
+        <f t="array" ref="D80">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A80),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>6600</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="8">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="10">
         <v>32402601800</v>
       </c>
-      <c r="B81" s="22" t="s">
+      <c r="B81" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="9">
         <v>1</v>
       </c>
-      <c r="D81">
-        <f>_xlfn.XLOOKUP(A81, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>4500</v>
-      </c>
-      <c r="E81" cm="1">
-        <f t="array" ref="E81">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A81),
+      <c r="D81" s="11" cm="1">
+        <f t="array" ref="D81">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A81),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>4500</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="8">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="10">
         <v>271921002614</v>
       </c>
-      <c r="B82" s="22" t="s">
+      <c r="B82" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="9">
         <v>1</v>
       </c>
-      <c r="D82">
-        <f>_xlfn.XLOOKUP(A82, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>2000</v>
-      </c>
-      <c r="E82" cm="1">
-        <f t="array" ref="E82">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A82),
+      <c r="D82" s="11" cm="1">
+        <f t="array" ref="D82">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A82),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="8">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="10">
         <v>325721000056</v>
       </c>
-      <c r="B83" s="22" t="s">
+      <c r="B83" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="9">
         <v>1</v>
       </c>
-      <c r="D83">
-        <f>_xlfn.XLOOKUP(A83, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>8500</v>
-      </c>
-      <c r="E83" cm="1">
-        <f t="array" ref="E83">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A83),
+      <c r="D83" s="11" cm="1">
+        <f t="array" ref="D83">LOOKUP(2,1/([1]VEPL_SMARTSOLUTION_DTP_INR!C$2:C$10000=A83),
          [1]VEPL_SMARTSOLUTION_DTP_INR!K$2:K$10000)</f>
         <v>8500</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="8" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B84" s="22" t="s">
+      <c r="B84" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="16">
         <v>1</v>
       </c>
-      <c r="D84" t="str">
-        <f>_xlfn.XLOOKUP(A84, [1]VEPL_SMARTSOLUTION_DTP_INR!C:C, [1]VEPL_SMARTSOLUTION_DTP_INR!K:K, "Not Found")</f>
-        <v>Not Found</v>
-      </c>
-      <c r="E84">
+      <c r="D84" s="17">
         <v>0</v>
       </c>
     </row>

</xml_diff>